<commit_message>
last job date added
</commit_message>
<xml_diff>
--- a/Database ChatGPT (1).xlsx
+++ b/Database ChatGPT (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\llm-examples\Chatbot-UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C732245D-7DE9-4657-861A-F2C4837B9F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBB2040-C1B3-444F-9C46-23436D7785AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Data</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>www.tracking.com</t>
+  </si>
+  <si>
+    <t>Last Job Date</t>
+  </si>
+  <si>
+    <t>January 1st 2022</t>
   </si>
 </sst>
 </file>
@@ -185,13 +191,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,7 +421,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -569,6 +576,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>

</xml_diff>